<commit_message>
added first gradCam working only on last fold
</commit_message>
<xml_diff>
--- a/Train_scripts/Excels/IF score.xlsx
+++ b/Train_scripts/Excels/IF score.xlsx
@@ -1854,7 +1854,7 @@
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>